<commit_message>
Recursive Search by name component
</commit_message>
<xml_diff>
--- a/Data/usernames.xlsx
+++ b/Data/usernames.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1469C89D-BF3C-4DDC-8892-9BE2ACE737EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05372AA5-5611-4783-880D-A391639BF89D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -30,12 +30,18 @@
   <si>
     <t>breedy_marvin</t>
   </si>
+  <si>
+    <t>realangelplein</t>
+  </si>
+  <si>
+    <t>uniquely_henrietta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,9 +50,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF262626"/>
-      <name val="Var(--font-family-system)"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,9 +80,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,34 +361,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Catered for the private account exception
</commit_message>
<xml_diff>
--- a/Data/usernames.xlsx
+++ b/Data/usernames.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2809EA56-4908-4165-A1B5-DF8BEC27053B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86811F0-E9CC-41B2-84BD-2AEB3AB6CC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>e.v.e83</t>
+  </si>
+  <si>
+    <t>uniquely_henrietta</t>
   </si>
 </sst>
 </file>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,16 +379,21 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>